<commit_message>
corrigido print de exemplo
</commit_message>
<xml_diff>
--- a/2em/2DES/01-bcd/aula10/exercicios/exercicio4_parcelas.xlsx
+++ b/2em/2DES/01-bcd/aula10/exercicios/exercicio4_parcelas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2022\2des\bcd\aula03\exercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wellifabio\sesi2024\2em\2DES\01-bcd\aula10\exercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4E33BC-4B66-4AF0-BBF1-EE545ACE53DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C7302-8A14-441F-A4D3-948329AE2230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68435E5F-DC9A-48F7-82EF-04866506E219}"/>
   </bookViews>
@@ -19,16 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -564,29 +554,29 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -636,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -686,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -736,7 +726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -786,7 +776,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -836,7 +826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -886,7 +876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -936,7 +926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -986,7 +976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1036,7 +1026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1086,7 +1076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1136,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1186,7 +1176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1236,7 +1226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1286,7 +1276,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1336,7 +1326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1386,7 +1376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1436,7 +1426,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1486,7 +1476,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1536,7 +1526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1586,7 +1576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1636,7 +1626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1686,7 +1676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1736,7 +1726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1786,7 +1776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1836,7 +1826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1886,7 +1876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1936,7 +1926,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1986,7 +1976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -2036,7 +2026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
@@ -2086,7 +2076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>7</v>
       </c>

</xml_diff>